<commit_message>
avitodata замена for на gen
</commit_message>
<xml_diff>
--- a/make_xl/data_xl/comp armchair.xlsx
+++ b/make_xl/data_xl/comp armchair.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\PycharmProjects\Tabels\make_xl\data_xl\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51C3DA8-F7CA-4AAC-A7D1-232A64EA5B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -903,6 +897,15 @@
     <t>https://disk.yandex.ru/i/UiSbbITJzTBOqw | https://disk.yandex.ru/i/BSwbfy6jE64Kpw | https://disk.yandex.ru/i/ut-HyMgP6ytXEA | https://disk.yandex.ru/i/P3f-5y7REJLEdg | https://disk.yandex.ru/i/E9s-9RthI59j8A | https://disk.yandex.ru/i/dKX_to5o7-PsSw | https://disk.yandex.ru/i/Rv74BQHjuHKSMg | https://disk.yandex.ru/i/JQfnVykq74XMLw | https://disk.yandex.ru/i/AFuhZxtmexdrmQ</t>
   </si>
   <si>
+    <t>https://disk.yandex.ru/i/bZpvYLgJkQeS5A | https://disk.yandex.ru/i/pQd-PGVs48AaIw | https://disk.yandex.ru/i/suuO6PTkZXJdwg | https://disk.yandex.ru/i/fHcjrSdVZpBP4w | https://disk.yandex.ru/i/JCCBmfu4mVBVKA | https://disk.yandex.ru/i/KSs7yEVXrQvtdg | https://disk.yandex.ru/i/b-JXSfrfJd4nhw | https://disk.yandex.ru/i/MCBY2S-TBrV2-A | https://disk.yandex.ru/i/jyeamFEdpJUNuA</t>
+  </si>
+  <si>
+    <t>https://disk.yandex.ru/i/zs1LO9iUDpfvJA | https://disk.yandex.ru/i/4XJto5aU9Pk5Qw | https://disk.yandex.ru/i/RW2frD43bhg6dA | https://disk.yandex.ru/i/i9uwNxDWupMaCg | https://disk.yandex.ru/i/2GcC1EzIDr7XHQ | https://disk.yandex.ru/i/WjREaYhYzBzk1Q | https://disk.yandex.ru/i/MFqy3a-nWEK21g | https://disk.yandex.ru/i/zKc5FfCGsSjQ2g | https://disk.yandex.ru/i/auG_5U6jJCE9OQ | https://disk.yandex.ru/i/flJEu_19ssvBBA</t>
+  </si>
+  <si>
+    <t>https://disk.yandex.ru/i/mO9zE0LznQaB8Q | https://disk.yandex.ru/i/rJG_GF3r4N8AmQ | https://disk.yandex.ru/i/p8UIxRy-jOuMng | https://disk.yandex.ru/i/2TEYu1-sI1QWQQ | https://disk.yandex.ru/i/rtiJTkhJ4__RNw | https://disk.yandex.ru/i/g7IeZQAmbGDzBQ | https://disk.yandex.ru/i/8KWCRYxO03XtgA</t>
+  </si>
+  <si>
     <t>https://youtu.be/ycYx204IpKc?si=5z8-v1fOQP2SdfR_</t>
   </si>
   <si>
@@ -1021,22 +1024,13 @@
   </si>
   <si>
     <t>Ткань | Сетка</t>
-  </si>
-  <si>
-    <t>https://disk.yandex.ru/i/bZpvYLgJkQeS5A | https://disk.yandex.ru/i/pQd-PGVs48AaIw | https://disk.yandex.ru/i/suuO6PTkZXJdwg | https://disk.yandex.ru/i/fHcjrSdVZpBP4w | https://disk.yandex.ru/i/JCCBmfu4mVBVKA | https://disk.yandex.ru/i/KSs7yEVXrQvtdg | https://disk.yandex.ru/i/b-JXSfrfJd4nhw | https://disk.yandex.ru/i/MCBY2S-TBrV2-A | https://disk.yandex.ru/i/jyeamFEdpJUNuA</t>
-  </si>
-  <si>
-    <t>https://disk.yandex.ru/i/zs1LO9iUDpfvJA | https://disk.yandex.ru/i/4XJto5aU9Pk5Qw | https://disk.yandex.ru/i/RW2frD43bhg6dA | https://disk.yandex.ru/i/i9uwNxDWupMaCg | https://disk.yandex.ru/i/2GcC1EzIDr7XHQ | https://disk.yandex.ru/i/WjREaYhYzBzk1Q | https://disk.yandex.ru/i/MFqy3a-nWEK21g | https://disk.yandex.ru/i/zKc5FfCGsSjQ2g | https://disk.yandex.ru/i/auG_5U6jJCE9OQ | https://disk.yandex.ru/i/flJEu_19ssvBBA</t>
-  </si>
-  <si>
-    <t>https://disk.yandex.ru/i/mO9zE0LznQaB8Q | https://disk.yandex.ru/i/rJG_GF3r4N8AmQ | https://disk.yandex.ru/i/p8UIxRy-jOuMng | https://disk.yandex.ru/i/2TEYu1-sI1QWQQ | https://disk.yandex.ru/i/rtiJTkhJ4__RNw | https://disk.yandex.ru/i/g7IeZQAmbGDzBQ | https://disk.yandex.ru/i/8KWCRYxO03XtgA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1107,26 +1101,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1164,9 +1150,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1198,27 +1184,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1250,27 +1218,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1443,16 +1393,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AV28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1598,7 +1546,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1615,31 +1563,31 @@
         <v>90</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AC2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="AG2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN2">
         <v>50</v>
@@ -1651,16 +1599,16 @@
         <v>50</v>
       </c>
       <c r="AQ2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="AR2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="AS2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AT2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="AU2">
         <v>30</v>
@@ -1669,7 +1617,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48">
       <c r="A3">
         <v>10031</v>
       </c>
@@ -1686,31 +1634,31 @@
         <v>91</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA3" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AC3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD3" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AG3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN3">
         <v>50</v>
@@ -1722,13 +1670,13 @@
         <v>50</v>
       </c>
       <c r="AQ3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="AS3" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AT3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AU3">
         <v>31</v>
@@ -1737,7 +1685,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48">
       <c r="A4">
         <v>10301</v>
       </c>
@@ -1754,31 +1702,31 @@
         <v>92</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AC4" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD4" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE4" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AG4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH4" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN4">
         <v>45</v>
@@ -1790,16 +1738,16 @@
         <v>40</v>
       </c>
       <c r="AQ4" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="AR4" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AS4" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AT4" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AU4">
         <v>30</v>
@@ -1808,7 +1756,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48">
       <c r="A5">
         <v>10301</v>
       </c>
@@ -1825,31 +1773,31 @@
         <v>93</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S5" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB5" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AC5" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD5" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE5" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AG5" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH5" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN5">
         <v>48</v>
@@ -1861,16 +1809,16 @@
         <v>50</v>
       </c>
       <c r="AQ5" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="AR5" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AS5" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AT5" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AU5">
         <v>30</v>
@@ -1879,7 +1827,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48">
       <c r="A6">
         <v>10301</v>
       </c>
@@ -1896,31 +1844,31 @@
         <v>93</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S6" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA6" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB6" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AC6" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD6" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE6" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AG6" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH6" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN6">
         <v>50</v>
@@ -1932,13 +1880,13 @@
         <v>50</v>
       </c>
       <c r="AQ6" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="AS6" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AT6" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AU6">
         <v>30</v>
@@ -1947,7 +1895,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48">
       <c r="A7">
         <v>10302</v>
       </c>
@@ -1964,31 +1912,31 @@
         <v>94</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S7" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA7" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB7" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AC7" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AG7" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH7" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN7">
         <v>45</v>
@@ -2000,16 +1948,16 @@
         <v>50</v>
       </c>
       <c r="AQ7" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="AR7" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="AS7" t="s">
+        <v>153</v>
+      </c>
+      <c r="AT7" t="s">
         <v>150</v>
-      </c>
-      <c r="AT7" t="s">
-        <v>147</v>
       </c>
       <c r="AU7">
         <v>30</v>
@@ -2018,7 +1966,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48">
       <c r="A8">
         <v>10310</v>
       </c>
@@ -2035,31 +1983,31 @@
         <v>95</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S8" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA8" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB8" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AC8" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD8" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE8" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="AG8" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH8" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN8">
         <v>48</v>
@@ -2071,16 +2019,16 @@
         <v>45</v>
       </c>
       <c r="AQ8" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="AR8" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="AS8" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AT8" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="AU8">
         <v>30</v>
@@ -2089,7 +2037,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48">
       <c r="A9">
         <v>10316</v>
       </c>
@@ -2106,31 +2054,31 @@
         <v>96</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S9" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA9" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB9" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AC9" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD9" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE9" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="AG9" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH9" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN9">
         <v>48</v>
@@ -2142,16 +2090,16 @@
         <v>50</v>
       </c>
       <c r="AQ9" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="AR9" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="AS9" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AT9" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="AU9">
         <v>30</v>
@@ -2160,7 +2108,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48">
       <c r="A10">
         <v>10316</v>
       </c>
@@ -2177,31 +2125,31 @@
         <v>97</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S10" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA10" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB10" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AC10" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD10" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE10" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AG10" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH10" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN10">
         <v>50</v>
@@ -2213,13 +2161,13 @@
         <v>50</v>
       </c>
       <c r="AQ10" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="AS10" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AT10" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="AU10">
         <v>30</v>
@@ -2228,7 +2176,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:48">
       <c r="A11">
         <v>10317</v>
       </c>
@@ -2245,31 +2193,31 @@
         <v>98</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S11" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA11" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB11" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AC11" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD11" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE11" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="AG11" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH11" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN11">
         <v>50</v>
@@ -2281,16 +2229,16 @@
         <v>48</v>
       </c>
       <c r="AQ11" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="AR11" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="AS11" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AT11" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="AU11">
         <v>30</v>
@@ -2299,7 +2247,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:48">
       <c r="A12">
         <v>10336</v>
       </c>
@@ -2316,31 +2264,31 @@
         <v>99</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S12" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA12" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB12" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AC12" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD12" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE12" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="AG12" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH12" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN12">
         <v>48</v>
@@ -2352,16 +2300,16 @@
         <v>50</v>
       </c>
       <c r="AQ12" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="AR12" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="AS12" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AT12" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="AU12">
         <v>31</v>
@@ -2370,7 +2318,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48">
       <c r="A13">
         <v>10368</v>
       </c>
@@ -2387,31 +2335,31 @@
         <v>100</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S13" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA13" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB13" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AC13" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD13" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE13" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AG13" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH13" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN13">
         <v>50</v>
@@ -2423,16 +2371,16 @@
         <v>50</v>
       </c>
       <c r="AQ13" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="AR13" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="AS13" t="s">
+        <v>153</v>
+      </c>
+      <c r="AT13" t="s">
         <v>150</v>
-      </c>
-      <c r="AT13" t="s">
-        <v>147</v>
       </c>
       <c r="AU13">
         <v>30</v>
@@ -2441,7 +2389,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48">
       <c r="A14">
         <v>10371</v>
       </c>
@@ -2458,31 +2406,31 @@
         <v>101</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S14" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA14" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB14" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AC14" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD14" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE14" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AG14" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH14" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN14">
         <v>50</v>
@@ -2494,16 +2442,16 @@
         <v>50</v>
       </c>
       <c r="AQ14" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="AR14" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS14" t="s">
+        <v>153</v>
+      </c>
+      <c r="AT14" t="s">
         <v>148</v>
-      </c>
-      <c r="AS14" t="s">
-        <v>150</v>
-      </c>
-      <c r="AT14" t="s">
-        <v>145</v>
       </c>
       <c r="AU14">
         <v>30</v>
@@ -2512,7 +2460,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48">
       <c r="A15">
         <v>10420</v>
       </c>
@@ -2529,31 +2477,31 @@
         <v>102</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S15" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA15" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB15" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AC15" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD15" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE15" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="AG15" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH15" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN15">
         <v>50</v>
@@ -2565,16 +2513,16 @@
         <v>50</v>
       </c>
       <c r="AQ15" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AR15" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="AS15" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AT15" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AU15">
         <v>30</v>
@@ -2583,7 +2531,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48">
       <c r="A16">
         <v>10424</v>
       </c>
@@ -2600,31 +2548,31 @@
         <v>103</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S16" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA16" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB16" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AC16" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD16" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE16" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AG16" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH16" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN16">
         <v>50</v>
@@ -2636,16 +2584,16 @@
         <v>50</v>
       </c>
       <c r="AQ16" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="AR16" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="AS16" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AT16" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="AU16">
         <v>30</v>
@@ -2654,7 +2602,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:48">
       <c r="A17">
         <v>10443</v>
       </c>
@@ -2671,31 +2619,31 @@
         <v>104</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S17" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA17" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB17" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AC17" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD17" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE17" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AG17" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN17">
         <v>55</v>
@@ -2707,16 +2655,16 @@
         <v>50</v>
       </c>
       <c r="AQ17" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="AR17" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="AS17" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AT17" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="AU17">
         <v>35</v>
@@ -2725,7 +2673,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:48">
       <c r="A18">
         <v>10460</v>
       </c>
@@ -2742,31 +2690,31 @@
         <v>105</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S18" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA18" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB18" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AC18" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD18" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE18" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AG18" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH18" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN18">
         <v>48</v>
@@ -2778,16 +2726,16 @@
         <v>50</v>
       </c>
       <c r="AQ18" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="AR18" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="AS18" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AT18" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="AU18">
         <v>30</v>
@@ -2796,7 +2744,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:48">
       <c r="A19">
         <v>10480</v>
       </c>
@@ -2813,31 +2761,31 @@
         <v>106</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S19" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA19" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB19" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AC19" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD19" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE19" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AG19" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH19" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN19">
         <v>50</v>
@@ -2849,16 +2797,16 @@
         <v>50</v>
       </c>
       <c r="AQ19" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="AR19" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="AS19" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AT19" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="AU19">
         <v>30</v>
@@ -2867,7 +2815,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:48">
       <c r="A20">
         <v>10494</v>
       </c>
@@ -2884,31 +2832,31 @@
         <v>107</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S20" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA20" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB20" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AC20" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD20" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE20" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AG20" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH20" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN20">
         <v>55</v>
@@ -2920,16 +2868,16 @@
         <v>50</v>
       </c>
       <c r="AQ20" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="AR20" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="AS20" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AT20" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="AU20">
         <v>30</v>
@@ -2938,7 +2886,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:48">
       <c r="A21">
         <v>10501</v>
       </c>
@@ -2955,31 +2903,31 @@
         <v>108</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S21" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA21" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB21" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AC21" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD21" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE21" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="AG21" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH21" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN21">
         <v>50</v>
@@ -2991,16 +2939,16 @@
         <v>53</v>
       </c>
       <c r="AQ21" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="AR21" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="AS21" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AT21" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="AU21">
         <v>30</v>
@@ -3009,7 +2957,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:48">
       <c r="A22">
         <v>10522</v>
       </c>
@@ -3026,31 +2974,31 @@
         <v>109</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S22" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB22" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AC22" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD22" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE22" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="AG22" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH22" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN22">
         <v>50</v>
@@ -3062,13 +3010,13 @@
         <v>50</v>
       </c>
       <c r="AQ22" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="AS22" t="s">
+        <v>153</v>
+      </c>
+      <c r="AT22" t="s">
         <v>150</v>
-      </c>
-      <c r="AT22" t="s">
-        <v>147</v>
       </c>
       <c r="AU22">
         <v>30</v>
@@ -3077,7 +3025,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:48">
       <c r="A23">
         <v>10522</v>
       </c>
@@ -3094,31 +3042,31 @@
         <v>110</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S23" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA23" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB23" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AC23" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD23" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE23" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="AG23" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH23" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN23">
         <v>48</v>
@@ -3130,13 +3078,13 @@
         <v>50</v>
       </c>
       <c r="AQ23" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="AS23" t="s">
+        <v>153</v>
+      </c>
+      <c r="AT23" t="s">
         <v>150</v>
-      </c>
-      <c r="AT23" t="s">
-        <v>147</v>
       </c>
       <c r="AU23">
         <v>30</v>
@@ -3145,7 +3093,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:48">
       <c r="A24">
         <v>10532</v>
       </c>
@@ -3162,31 +3110,31 @@
         <v>111</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S24" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA24" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB24" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AC24" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD24" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE24" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="AG24" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH24" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN24">
         <v>48</v>
@@ -3198,13 +3146,13 @@
         <v>50</v>
       </c>
       <c r="AQ24" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="AS24" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AT24" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AU24">
         <v>30</v>
@@ -3213,7 +3161,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:48">
       <c r="A25">
         <v>10532</v>
       </c>
@@ -3230,31 +3178,31 @@
         <v>112</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S25" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA25" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB25" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AC25" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD25" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE25" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="AG25" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH25" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AN25">
         <v>48</v>
@@ -3266,13 +3214,13 @@
         <v>50</v>
       </c>
       <c r="AQ25" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="AS25" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AT25" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AU25">
         <v>30</v>
@@ -3281,7 +3229,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:48">
       <c r="A26">
         <v>10410</v>
       </c>
@@ -3295,46 +3243,46 @@
         <v>12000</v>
       </c>
       <c r="O26" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="S26" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>122</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>124</v>
+      </c>
+      <c r="AG26" t="s">
+        <v>132</v>
+      </c>
+      <c r="AH26" t="s">
+        <v>133</v>
+      </c>
+      <c r="AQ26" t="s">
+        <v>147</v>
+      </c>
+      <c r="AS26" t="s">
         <v>153</v>
       </c>
-      <c r="Q26" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="S26" t="s">
-        <v>114</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>115</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC26" t="s">
-        <v>118</v>
-      </c>
-      <c r="AD26" t="s">
-        <v>119</v>
-      </c>
-      <c r="AE26" t="s">
-        <v>121</v>
-      </c>
-      <c r="AG26" t="s">
-        <v>129</v>
-      </c>
-      <c r="AH26" t="s">
-        <v>130</v>
-      </c>
-      <c r="AQ26" t="s">
-        <v>144</v>
-      </c>
-      <c r="AS26" t="s">
-        <v>150</v>
-      </c>
       <c r="AT26" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
-    <row r="27" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:48">
       <c r="A27">
         <v>10301</v>
       </c>
@@ -3348,46 +3296,46 @@
         <v>2999</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S27" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA27" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB27" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AC27" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD27" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE27" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AG27" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH27" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AQ27" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="AS27" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AT27" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
-    <row r="28" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:48">
       <c r="A28">
         <v>10538</v>
       </c>
@@ -3401,98 +3349,101 @@
         <v>14999</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>155</v>
+        <v>115</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="S28" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AA28" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AB28" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AC28" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AD28" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AE28" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AG28" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AH28" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AQ28" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="AS28" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AT28" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="Q2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="O3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="Q3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="O4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="Q4" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="O5" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="Q5" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="O6" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="Q6" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="O7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="Q7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="O8" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="Q8" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="O9" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="Q9" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="O10" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="Q10" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="O11" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="Q11" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="O12" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="Q12" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="O13" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="Q13" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="O14" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="Q14" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="O15" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="Q15" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="O16" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="Q16" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="O17" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="Q17" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="O18" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="Q18" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="O19" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="Q19" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="O20" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="Q20" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="O21" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="Q21" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="O22" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="Q22" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="O23" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="Q23" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="O24" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="Q24" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="O25" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="Q25" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="Q26" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="Q27" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="Q28" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="O2" r:id="rId1"/>
+    <hyperlink ref="Q2" r:id="rId2"/>
+    <hyperlink ref="O3" r:id="rId3"/>
+    <hyperlink ref="Q3" r:id="rId4"/>
+    <hyperlink ref="O4" r:id="rId5"/>
+    <hyperlink ref="Q4" r:id="rId6"/>
+    <hyperlink ref="O5" r:id="rId7"/>
+    <hyperlink ref="Q5" r:id="rId8"/>
+    <hyperlink ref="O6" r:id="rId9"/>
+    <hyperlink ref="Q6" r:id="rId10"/>
+    <hyperlink ref="O7" r:id="rId11"/>
+    <hyperlink ref="Q7" r:id="rId12"/>
+    <hyperlink ref="O8" r:id="rId13"/>
+    <hyperlink ref="Q8" r:id="rId14"/>
+    <hyperlink ref="O9" r:id="rId15"/>
+    <hyperlink ref="Q9" r:id="rId16"/>
+    <hyperlink ref="O10" r:id="rId17"/>
+    <hyperlink ref="Q10" r:id="rId18"/>
+    <hyperlink ref="O11" r:id="rId19"/>
+    <hyperlink ref="Q11" r:id="rId20"/>
+    <hyperlink ref="O12" r:id="rId21"/>
+    <hyperlink ref="Q12" r:id="rId22"/>
+    <hyperlink ref="O13" r:id="rId23"/>
+    <hyperlink ref="Q13" r:id="rId24"/>
+    <hyperlink ref="O14" r:id="rId25"/>
+    <hyperlink ref="Q14" r:id="rId26"/>
+    <hyperlink ref="O15" r:id="rId27"/>
+    <hyperlink ref="Q15" r:id="rId28"/>
+    <hyperlink ref="O16" r:id="rId29"/>
+    <hyperlink ref="Q16" r:id="rId30"/>
+    <hyperlink ref="O17" r:id="rId31"/>
+    <hyperlink ref="Q17" r:id="rId32"/>
+    <hyperlink ref="O18" r:id="rId33"/>
+    <hyperlink ref="Q18" r:id="rId34"/>
+    <hyperlink ref="O19" r:id="rId35"/>
+    <hyperlink ref="Q19" r:id="rId36"/>
+    <hyperlink ref="O20" r:id="rId37"/>
+    <hyperlink ref="Q20" r:id="rId38"/>
+    <hyperlink ref="O21" r:id="rId39"/>
+    <hyperlink ref="Q21" r:id="rId40"/>
+    <hyperlink ref="O22" r:id="rId41"/>
+    <hyperlink ref="Q22" r:id="rId42"/>
+    <hyperlink ref="O23" r:id="rId43"/>
+    <hyperlink ref="Q23" r:id="rId44"/>
+    <hyperlink ref="O24" r:id="rId45"/>
+    <hyperlink ref="Q24" r:id="rId46"/>
+    <hyperlink ref="O25" r:id="rId47"/>
+    <hyperlink ref="Q25" r:id="rId48"/>
+    <hyperlink ref="O26" r:id="rId49"/>
+    <hyperlink ref="Q26" r:id="rId50"/>
+    <hyperlink ref="O27" r:id="rId51"/>
+    <hyperlink ref="Q27" r:id="rId52"/>
+    <hyperlink ref="O28" r:id="rId53"/>
+    <hyperlink ref="Q28" r:id="rId54"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>